<commit_message>
query by documents tested in top2vec
</commit_message>
<xml_diff>
--- a/Project_python/out/Top2vec/optimization_out.xlsx
+++ b/Project_python/out/Top2vec/optimization_out.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Sum total: x1:1.000|x2:0.726|x3:3.855|x4:0.670|x5:0.726|x6:0.687|x7:0.759|x8:1.000|x9:1.006|x10:1.000|x11:0.737|x12:1.000|x13:1.000|x14:0.968|x15:1.032|x16:0.835|x17:0.000</t>
+          <t>Sum total: x1:1.000|x2:0.726|x3:3.854|x4:0.670|x5:0.726|x6:0.687|x7:0.759|x8:1.000|x9:1.006|x10:1.000|x11:0.737|x12:1.000|x13:1.000|x14:0.968|x15:1.032|x16:0.835|x17:0.000</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -523,12 +523,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>10.976, 13.415</t>
+          <t>89.634, 92.073</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>87.267, 87.578</t>
+          <t>86.957, 87.267</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
testdataset revised, cleaned and relabelled
</commit_message>
<xml_diff>
--- a/Project_python/out/Top2vec/optimization_out.xlsx
+++ b/Project_python/out/Top2vec/optimization_out.xlsx
@@ -513,22 +513,22 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Sum total: x1:0.849|x2:1.000|x3:2.000|x4:1.000|x5:1.000|x6:1.000|x7:1.000|x8:1.000|x9:1.000|x10:1.151|x11:1.000|x12:1.000|x13:1.000|x14:1.000|x15:1.000|x16:1.000|x17:0.000</t>
+          <t>Sum total: x1:1.000|x2:1.000|x3:2.000|x4:1.000|x5:1.000|x6:1.000|x7:0.563|x8:1.000|x9:1.000|x10:1.000|x11:1.000|x12:0.437|x13:1.000|x14:1.000|x15:1.000|x16:1.000|x17:0.000</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1.000, 0.347</t>
+          <t>0.941, 0.380</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>88.710, 90.323</t>
+          <t>88.172, 89.247</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>100.000, 100.000</t>
+          <t>99.810, 99.810</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
top2vec -> continuos distribution
</commit_message>
<xml_diff>
--- a/Project_python/out/Top2vec/optimization_out.xlsx
+++ b/Project_python/out/Top2vec/optimization_out.xlsx
@@ -513,22 +513,22 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Sum total: x1:1.000|x2:1.000|x3:2.000|x4:1.000|x5:1.000|x6:1.000|x7:0.563|x8:1.000|x9:1.000|x10:1.000|x11:1.000|x12:0.437|x13:1.000|x14:1.000|x15:1.000|x16:1.000|x17:0.000</t>
+          <t>Sum total: x1:0.795|x2:0.957|x3:1.637|x4:1.035|x5:1.183|x6:0.966|x7:0.923|x8:1.041|x9:1.356|x10:0.970|x11:1.302|x12:1.121|x13:0.575|x14:0.574|x15:0.712|x16:0.854|x17:0.000</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.941, 0.380</t>
+          <t>0.941, 0.354</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>88.172, 89.247</t>
+          <t>68.280, 71.505</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>99.810, 99.810</t>
+          <t>82.343, 82.504</t>
         </is>
       </c>
     </row>

</xml_diff>